<commit_message>
V3 Consume list of emails
</commit_message>
<xml_diff>
--- a/bin/Debug/netcoreapp2.1/Input/Values.xlsx
+++ b/bin/Debug/netcoreapp2.1/Input/Values.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="248">
   <si>
     <t>actionGroupShortName</t>
   </si>
@@ -763,10 +763,16 @@
     <t>emailList</t>
   </si>
   <si>
-    <t>{
+    <t>[{
           "name": "NZME Dev Group",
           "email": "dotnetdevs@groups.nzme.co.nz"
-        }</t>
+        }]</t>
+  </si>
+  <si>
+    <t>[{
+          "name": "NZME Dev Group",
+          "email": "dotnetdevs@groups.nzme.co.nz"
+        },]</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,10 +1126,10 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73.5703125" customWidth="1"/>
+    <col min="10" max="10" width="51.7109375" customWidth="1"/>
     <col min="11" max="11" width="6.7109375" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
     <col min="13" max="13" width="24.5703125" customWidth="1"/>
@@ -1171,7 +1177,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1209,7 +1215,7 @@
         <v>33</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>